<commit_message>
Konzept überarbeitet, Dokumentation angelegt
</commit_message>
<xml_diff>
--- a/konzept/projektplan.xlsx
+++ b/konzept/projektplan.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="133">
   <si>
     <t>#</t>
   </si>
@@ -413,6 +413,12 @@
   </si>
   <si>
     <t>Soll-Stunde</t>
+  </si>
+  <si>
+    <t>4.0</t>
+  </si>
+  <si>
+    <t>Planung Vorgehen</t>
   </si>
 </sst>
 </file>
@@ -1007,7 +1013,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="123">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1191,6 +1197,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
@@ -1573,10 +1583,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:EH206"/>
+  <dimension ref="A1:EH207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+    <sheetView tabSelected="1" topLeftCell="C14" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3243,65 +3253,82 @@
       <c r="CQ32" s="16"/>
     </row>
     <row r="33" spans="1:109">
-      <c r="A33" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B33" t="s">
-        <v>105</v>
-      </c>
-      <c r="C33">
-        <v>3</v>
-      </c>
-      <c r="E33">
-        <v>3</v>
-      </c>
-      <c r="AT33" s="95"/>
-      <c r="AU33" s="93"/>
-      <c r="AV33" s="91"/>
+      <c r="A33" s="123" t="s">
+        <v>131</v>
+      </c>
+      <c r="B33" s="124" t="s">
+        <v>132</v>
+      </c>
+      <c r="AR33" s="68"/>
+      <c r="AS33" s="69"/>
+      <c r="AT33" s="70"/>
+      <c r="AU33" s="68"/>
+      <c r="AV33" s="68"/>
+      <c r="AW33" s="68"/>
+      <c r="AX33" s="68"/>
+      <c r="AY33" s="68"/>
+      <c r="AZ33" s="68"/>
+      <c r="BA33" s="68"/>
+      <c r="BB33" s="68"/>
+      <c r="BC33" s="68"/>
+      <c r="BD33" s="71"/>
+      <c r="BE33" s="68"/>
+      <c r="BF33" s="68"/>
+      <c r="BG33" s="68"/>
+      <c r="BH33" s="68"/>
+      <c r="BI33" s="68"/>
+      <c r="BJ33" s="68"/>
+      <c r="BK33" s="68"/>
+      <c r="BL33" s="68"/>
+      <c r="BM33" s="68"/>
+      <c r="BN33" s="68"/>
+      <c r="BO33" s="68"/>
       <c r="CM33" s="82"/>
       <c r="CQ33" s="16"/>
     </row>
     <row r="34" spans="1:109">
       <c r="A34" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B34" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C34">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E34">
-        <v>5</v>
-      </c>
-      <c r="AV34" s="94"/>
-      <c r="AW34" s="94"/>
+        <v>3</v>
+      </c>
+      <c r="AT34" s="95"/>
+      <c r="AU34" s="93"/>
+      <c r="AV34" s="91"/>
       <c r="CM34" s="82"/>
       <c r="CQ34" s="16"/>
     </row>
     <row r="35" spans="1:109">
       <c r="A35" s="1" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="B35" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C35">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E35">
-        <v>4</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="AV35" s="94"/>
       <c r="AW35" s="94"/>
       <c r="CM35" s="82"/>
       <c r="CQ35" s="16"/>
     </row>
     <row r="36" spans="1:109">
       <c r="A36" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B36" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C36">
         <v>4</v>
@@ -3309,90 +3336,103 @@
       <c r="E36">
         <v>4</v>
       </c>
-      <c r="BA36" s="96"/>
-      <c r="BB36" s="96"/>
+      <c r="AW36" s="94"/>
       <c r="CM36" s="82"/>
       <c r="CQ36" s="16"/>
     </row>
     <row r="37" spans="1:109">
       <c r="A37" s="1" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="B37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C37">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E37">
-        <v>5</v>
-      </c>
-      <c r="BC37" s="97"/>
-      <c r="BD37" s="98"/>
-      <c r="BH37" s="97"/>
+        <v>4</v>
+      </c>
+      <c r="BA37" s="96"/>
+      <c r="BB37" s="96"/>
       <c r="CM37" s="82"/>
       <c r="CQ37" s="16"/>
     </row>
     <row r="38" spans="1:109">
       <c r="A38" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B38" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C38">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E38">
-        <v>8</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="BC38" s="97"/>
+      <c r="BD38" s="98"/>
       <c r="BH38" s="97"/>
-      <c r="BI38" s="97"/>
-      <c r="BJ38" s="97"/>
-      <c r="BK38" s="97"/>
-      <c r="BO38" s="82"/>
-      <c r="BP38" s="91"/>
       <c r="CM38" s="82"/>
       <c r="CQ38" s="16"/>
     </row>
     <row r="39" spans="1:109">
       <c r="A39" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B39" t="s">
-        <v>87</v>
+        <v>114</v>
       </c>
       <c r="C39">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E39">
-        <v>3</v>
-      </c>
-      <c r="BO39" s="96"/>
-      <c r="BP39" s="96"/>
-      <c r="BQ39" s="91"/>
+        <v>8</v>
+      </c>
+      <c r="BH39" s="97"/>
+      <c r="BI39" s="97"/>
+      <c r="BJ39" s="97"/>
+      <c r="BK39" s="97"/>
+      <c r="BO39" s="82"/>
+      <c r="BP39" s="91"/>
       <c r="CM39" s="82"/>
       <c r="CQ39" s="16"/>
     </row>
     <row r="40" spans="1:109">
       <c r="A40" s="1" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="B40" t="s">
-        <v>113</v>
+        <v>87</v>
       </c>
       <c r="C40">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E40">
-        <v>2</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="BO40" s="96"/>
       <c r="BP40" s="96"/>
-      <c r="BQ40" s="96"/>
+      <c r="BQ40" s="91"/>
       <c r="CM40" s="82"/>
       <c r="CQ40" s="16"/>
     </row>
     <row r="41" spans="1:109">
+      <c r="A41" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B41" t="s">
+        <v>113</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="E41">
+        <v>2</v>
+      </c>
+      <c r="BP41" s="96"/>
+      <c r="BQ41" s="96"/>
       <c r="CM41" s="82"/>
       <c r="CQ41" s="16"/>
     </row>
@@ -3401,361 +3441,347 @@
       <c r="CQ42" s="16"/>
     </row>
     <row r="43" spans="1:109">
-      <c r="A43" s="8" t="s">
+      <c r="CM43" s="82"/>
+      <c r="CQ43" s="16"/>
+    </row>
+    <row r="44" spans="1:109">
+      <c r="A44" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="B43" s="9" t="s">
+      <c r="B44" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C43">
+      <c r="C44">
         <v>95</v>
       </c>
-      <c r="E43">
+      <c r="E44">
         <v>95</v>
       </c>
-      <c r="BM43" s="82"/>
-      <c r="BN43" s="82"/>
-      <c r="BO43" s="72"/>
-      <c r="BP43" s="72"/>
-      <c r="BQ43" s="72"/>
-      <c r="BR43" s="72"/>
-      <c r="BS43" s="72"/>
-      <c r="BT43" s="72"/>
-      <c r="BU43" s="72"/>
-      <c r="BV43" s="72"/>
-      <c r="BW43" s="73"/>
-      <c r="BX43" s="74"/>
-      <c r="BY43" s="72"/>
-      <c r="BZ43" s="72"/>
-      <c r="CA43" s="72"/>
-      <c r="CB43" s="72"/>
-      <c r="CC43" s="72"/>
-      <c r="CD43" s="72"/>
-      <c r="CE43" s="72"/>
-      <c r="CF43" s="72"/>
-      <c r="CG43" s="72"/>
-      <c r="CH43" s="72"/>
-      <c r="CI43" s="72"/>
-      <c r="CJ43" s="72"/>
-      <c r="CK43" s="72"/>
-      <c r="CL43" s="72"/>
-      <c r="CM43" s="72"/>
-      <c r="CN43" s="72"/>
-      <c r="CO43" s="72"/>
-      <c r="CP43" s="72"/>
-      <c r="CQ43" s="72"/>
-      <c r="CR43" s="105"/>
-      <c r="CS43" s="105"/>
-      <c r="CT43" s="105"/>
-      <c r="CU43" s="105"/>
-      <c r="CV43" s="105"/>
-      <c r="CW43" s="105"/>
-      <c r="CX43" s="105"/>
-      <c r="CY43" s="105"/>
-      <c r="CZ43" s="105"/>
-      <c r="DA43" s="105"/>
-      <c r="DB43" s="106"/>
-      <c r="DC43" s="107"/>
-      <c r="DD43" s="105"/>
-      <c r="DE43" s="105"/>
-    </row>
-    <row r="44" spans="1:109">
-      <c r="A44" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="BO44" s="102"/>
-      <c r="BP44" s="102"/>
-      <c r="BQ44" s="102"/>
-      <c r="BR44" s="102"/>
-      <c r="BS44" s="82"/>
-      <c r="CM44" s="82"/>
-      <c r="CQ44" s="16"/>
+      <c r="BM44" s="82"/>
+      <c r="BN44" s="82"/>
+      <c r="BO44" s="72"/>
+      <c r="BP44" s="72"/>
+      <c r="BQ44" s="72"/>
+      <c r="BR44" s="72"/>
+      <c r="BS44" s="72"/>
+      <c r="BT44" s="72"/>
+      <c r="BU44" s="72"/>
+      <c r="BV44" s="72"/>
+      <c r="BW44" s="73"/>
+      <c r="BX44" s="74"/>
+      <c r="BY44" s="72"/>
+      <c r="BZ44" s="72"/>
+      <c r="CA44" s="72"/>
+      <c r="CB44" s="72"/>
+      <c r="CC44" s="72"/>
+      <c r="CD44" s="72"/>
+      <c r="CE44" s="72"/>
+      <c r="CF44" s="72"/>
+      <c r="CG44" s="72"/>
+      <c r="CH44" s="72"/>
+      <c r="CI44" s="72"/>
+      <c r="CJ44" s="72"/>
+      <c r="CK44" s="72"/>
+      <c r="CL44" s="72"/>
+      <c r="CM44" s="72"/>
+      <c r="CN44" s="72"/>
+      <c r="CO44" s="72"/>
+      <c r="CP44" s="72"/>
+      <c r="CQ44" s="72"/>
+      <c r="CR44" s="105"/>
+      <c r="CS44" s="105"/>
+      <c r="CT44" s="105"/>
+      <c r="CU44" s="105"/>
+      <c r="CV44" s="105"/>
+      <c r="CW44" s="105"/>
+      <c r="CX44" s="105"/>
+      <c r="CY44" s="105"/>
+      <c r="CZ44" s="105"/>
+      <c r="DA44" s="105"/>
+      <c r="DB44" s="106"/>
+      <c r="DC44" s="107"/>
+      <c r="DD44" s="105"/>
+      <c r="DE44" s="105"/>
     </row>
     <row r="45" spans="1:109">
       <c r="A45" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="BU45" s="102"/>
-      <c r="BV45" s="102"/>
-      <c r="BW45" s="103"/>
-      <c r="BX45" s="104"/>
-      <c r="BY45" s="102"/>
+        <v>89</v>
+      </c>
+      <c r="BO45" s="102"/>
+      <c r="BP45" s="102"/>
+      <c r="BQ45" s="102"/>
+      <c r="BR45" s="102"/>
+      <c r="BS45" s="82"/>
       <c r="CM45" s="82"/>
       <c r="CQ45" s="16"/>
     </row>
     <row r="46" spans="1:109">
       <c r="A46" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="CB46" s="102"/>
-      <c r="CC46" s="102"/>
-      <c r="CD46" s="102"/>
-      <c r="CE46" s="102"/>
-      <c r="CF46" s="102"/>
+        <v>91</v>
+      </c>
+      <c r="BU46" s="102"/>
+      <c r="BV46" s="102"/>
+      <c r="BW46" s="103"/>
+      <c r="BX46" s="104"/>
+      <c r="BY46" s="102"/>
       <c r="CM46" s="82"/>
       <c r="CQ46" s="16"/>
     </row>
     <row r="47" spans="1:109">
       <c r="A47" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="CI47" s="102"/>
-      <c r="CJ47" s="102"/>
-      <c r="CK47" s="102"/>
-      <c r="CL47" s="102"/>
-      <c r="CM47" s="102"/>
+        <v>92</v>
+      </c>
+      <c r="CB47" s="102"/>
+      <c r="CC47" s="102"/>
+      <c r="CD47" s="102"/>
+      <c r="CE47" s="102"/>
+      <c r="CF47" s="102"/>
+      <c r="CM47" s="82"/>
       <c r="CQ47" s="16"/>
     </row>
     <row r="48" spans="1:109">
       <c r="A48" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="CI48" s="102"/>
+      <c r="CJ48" s="102"/>
+      <c r="CK48" s="102"/>
+      <c r="CL48" s="102"/>
+      <c r="CM48" s="102"/>
+      <c r="CQ48" s="16"/>
+    </row>
+    <row r="49" spans="1:133">
+      <c r="A49" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>95</v>
       </c>
-      <c r="C48">
+      <c r="C49">
         <v>30</v>
       </c>
-      <c r="E48">
+      <c r="E49">
         <v>30</v>
       </c>
-      <c r="CM48" s="82"/>
-      <c r="CQ48" s="16"/>
-    </row>
-    <row r="49" spans="1:133">
-      <c r="CM49" s="102"/>
-      <c r="CN49" s="102"/>
-      <c r="CO49" s="102"/>
-      <c r="CP49" s="102"/>
-      <c r="CQ49" s="102"/>
+      <c r="CM49" s="82"/>
+      <c r="CQ49" s="16"/>
     </row>
     <row r="50" spans="1:133">
-      <c r="A50" s="10" t="s">
+      <c r="CM50" s="102"/>
+      <c r="CN50" s="102"/>
+      <c r="CO50" s="102"/>
+      <c r="CP50" s="102"/>
+      <c r="CQ50" s="102"/>
+    </row>
+    <row r="51" spans="1:133">
+      <c r="A51" s="10" t="s">
         <v>90</v>
       </c>
-      <c r="B50" s="11" t="s">
+      <c r="B51" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="AR50" s="75"/>
-      <c r="AS50" s="76"/>
-      <c r="AT50" s="77"/>
-      <c r="AU50" s="75"/>
-      <c r="AV50" s="75"/>
-      <c r="AW50" s="75"/>
-      <c r="AX50" s="75"/>
-      <c r="AY50" s="75"/>
-      <c r="AZ50" s="75"/>
-      <c r="BA50" s="75"/>
-      <c r="BB50" s="75"/>
-      <c r="BC50" s="75"/>
-      <c r="BD50" s="78"/>
-      <c r="BE50" s="75"/>
-      <c r="BF50" s="75"/>
-      <c r="BG50" s="75"/>
-      <c r="BH50" s="75"/>
-      <c r="BI50" s="75"/>
-      <c r="BJ50" s="75"/>
-      <c r="BK50" s="75"/>
-      <c r="BL50" s="75"/>
-      <c r="BM50" s="75"/>
-      <c r="BN50" s="75"/>
-      <c r="BO50" s="75"/>
-      <c r="BP50" s="75"/>
-      <c r="BQ50" s="75"/>
-      <c r="BR50" s="75"/>
-      <c r="BS50" s="75"/>
-      <c r="BT50" s="75"/>
-      <c r="BU50" s="75"/>
-      <c r="BV50" s="75"/>
-      <c r="BW50" s="76"/>
-      <c r="BX50" s="77"/>
-      <c r="BY50" s="75"/>
-      <c r="BZ50" s="75"/>
-      <c r="CA50" s="75"/>
-      <c r="CB50" s="75"/>
-      <c r="CC50" s="75"/>
-      <c r="CD50" s="75"/>
-      <c r="CE50" s="75"/>
-      <c r="CF50" s="75"/>
-      <c r="CG50" s="75"/>
-      <c r="CH50" s="75"/>
-      <c r="CI50" s="75"/>
-      <c r="CJ50" s="75"/>
-      <c r="CK50" s="75"/>
-      <c r="CL50" s="75"/>
-      <c r="CM50" s="75"/>
-      <c r="CN50" s="75"/>
-      <c r="CO50" s="75"/>
-      <c r="CP50" s="75"/>
-      <c r="CQ50" s="75"/>
-      <c r="CR50" s="75"/>
-      <c r="CS50" s="75"/>
-      <c r="CT50" s="75"/>
-      <c r="CU50" s="75"/>
-      <c r="CV50" s="75"/>
-      <c r="CW50" s="75"/>
-      <c r="CX50" s="75"/>
-      <c r="CY50" s="75"/>
-      <c r="CZ50" s="75"/>
-      <c r="DA50" s="75"/>
-      <c r="DB50" s="76"/>
-      <c r="DC50" s="77"/>
-      <c r="DD50" s="75"/>
-      <c r="DE50" s="75"/>
-      <c r="DF50" s="75"/>
-      <c r="DG50" s="75"/>
-      <c r="DH50" s="75"/>
-      <c r="DI50" s="75"/>
-      <c r="DJ50" s="75"/>
-      <c r="DK50" s="75"/>
-      <c r="DL50" s="75"/>
-      <c r="DM50" s="75"/>
-      <c r="DN50" s="75"/>
-      <c r="DO50" s="75"/>
-    </row>
-    <row r="51" spans="1:133">
-      <c r="A51" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="B51" t="s">
-        <v>126</v>
-      </c>
-      <c r="C51">
-        <v>2</v>
-      </c>
-      <c r="E51">
-        <v>3</v>
-      </c>
-      <c r="AW51" s="84"/>
-      <c r="BA51" s="84"/>
-      <c r="BB51" s="84"/>
-      <c r="CM51" s="82"/>
-      <c r="CQ51" s="16"/>
+      <c r="AR51" s="75"/>
+      <c r="AS51" s="76"/>
+      <c r="AT51" s="77"/>
+      <c r="AU51" s="75"/>
+      <c r="AV51" s="75"/>
+      <c r="AW51" s="75"/>
+      <c r="AX51" s="75"/>
+      <c r="AY51" s="75"/>
+      <c r="AZ51" s="75"/>
+      <c r="BA51" s="75"/>
+      <c r="BB51" s="75"/>
+      <c r="BC51" s="75"/>
+      <c r="BD51" s="78"/>
+      <c r="BE51" s="75"/>
+      <c r="BF51" s="75"/>
+      <c r="BG51" s="75"/>
+      <c r="BH51" s="75"/>
+      <c r="BI51" s="75"/>
+      <c r="BJ51" s="75"/>
+      <c r="BK51" s="75"/>
+      <c r="BL51" s="75"/>
+      <c r="BM51" s="75"/>
+      <c r="BN51" s="75"/>
+      <c r="BO51" s="75"/>
+      <c r="BP51" s="75"/>
+      <c r="BQ51" s="75"/>
+      <c r="BR51" s="75"/>
+      <c r="BS51" s="75"/>
+      <c r="BT51" s="75"/>
+      <c r="BU51" s="75"/>
+      <c r="BV51" s="75"/>
+      <c r="BW51" s="76"/>
+      <c r="BX51" s="77"/>
+      <c r="BY51" s="75"/>
+      <c r="BZ51" s="75"/>
+      <c r="CA51" s="75"/>
+      <c r="CB51" s="75"/>
+      <c r="CC51" s="75"/>
+      <c r="CD51" s="75"/>
+      <c r="CE51" s="75"/>
+      <c r="CF51" s="75"/>
+      <c r="CG51" s="75"/>
+      <c r="CH51" s="75"/>
+      <c r="CI51" s="75"/>
+      <c r="CJ51" s="75"/>
+      <c r="CK51" s="75"/>
+      <c r="CL51" s="75"/>
+      <c r="CM51" s="75"/>
+      <c r="CN51" s="75"/>
+      <c r="CO51" s="75"/>
+      <c r="CP51" s="75"/>
+      <c r="CQ51" s="75"/>
+      <c r="CR51" s="75"/>
+      <c r="CS51" s="75"/>
+      <c r="CT51" s="75"/>
+      <c r="CU51" s="75"/>
+      <c r="CV51" s="75"/>
+      <c r="CW51" s="75"/>
+      <c r="CX51" s="75"/>
+      <c r="CY51" s="75"/>
+      <c r="CZ51" s="75"/>
+      <c r="DA51" s="75"/>
+      <c r="DB51" s="76"/>
+      <c r="DC51" s="77"/>
+      <c r="DD51" s="75"/>
+      <c r="DE51" s="75"/>
+      <c r="DF51" s="75"/>
+      <c r="DG51" s="75"/>
+      <c r="DH51" s="75"/>
+      <c r="DI51" s="75"/>
+      <c r="DJ51" s="75"/>
+      <c r="DK51" s="75"/>
+      <c r="DL51" s="75"/>
+      <c r="DM51" s="75"/>
+      <c r="DN51" s="75"/>
+      <c r="DO51" s="75"/>
     </row>
     <row r="52" spans="1:133">
       <c r="A52" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B52" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C52">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="E52">
-        <v>45</v>
-      </c>
-      <c r="BD52" s="85"/>
-      <c r="BH52" s="84"/>
-      <c r="BI52" s="84"/>
-      <c r="BJ52" s="84"/>
-      <c r="BK52" s="84"/>
-      <c r="BO52" s="84"/>
-      <c r="BP52" s="84"/>
-      <c r="BQ52" s="84"/>
-      <c r="BR52" s="84"/>
-      <c r="BS52" s="84"/>
-      <c r="BV52" s="84"/>
-      <c r="BW52" s="86"/>
-      <c r="BX52" s="87"/>
-      <c r="BY52" s="84"/>
-      <c r="CC52" s="84"/>
-      <c r="CD52" s="84"/>
-      <c r="CE52" s="84"/>
-      <c r="CF52" s="84"/>
-      <c r="CJ52" s="84"/>
-      <c r="CK52" s="84"/>
-      <c r="CL52" s="84"/>
-      <c r="CM52" s="84"/>
-      <c r="CP52" s="84"/>
-      <c r="CQ52" s="84"/>
-      <c r="CR52" s="84"/>
-      <c r="CS52" s="84"/>
-      <c r="CT52" s="84"/>
-      <c r="CW52" s="84"/>
-      <c r="CX52" s="84"/>
+        <v>3</v>
+      </c>
+      <c r="AW52" s="84"/>
+      <c r="BA52" s="84"/>
+      <c r="BB52" s="84"/>
+      <c r="CM52" s="82"/>
+      <c r="CQ52" s="16"/>
     </row>
     <row r="53" spans="1:133">
       <c r="A53" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B53" t="s">
+        <v>127</v>
+      </c>
+      <c r="C53">
+        <v>45</v>
+      </c>
+      <c r="E53">
+        <v>45</v>
+      </c>
+      <c r="BD53" s="85"/>
+      <c r="BH53" s="84"/>
+      <c r="BI53" s="84"/>
+      <c r="BJ53" s="84"/>
+      <c r="BK53" s="84"/>
+      <c r="BO53" s="84"/>
+      <c r="BP53" s="84"/>
+      <c r="BQ53" s="84"/>
+      <c r="BR53" s="84"/>
+      <c r="BS53" s="84"/>
+      <c r="BV53" s="84"/>
+      <c r="BW53" s="86"/>
+      <c r="BX53" s="87"/>
+      <c r="BY53" s="84"/>
+      <c r="CC53" s="84"/>
+      <c r="CD53" s="84"/>
+      <c r="CE53" s="84"/>
+      <c r="CF53" s="84"/>
+      <c r="CJ53" s="84"/>
+      <c r="CK53" s="84"/>
+      <c r="CL53" s="84"/>
+      <c r="CM53" s="84"/>
+      <c r="CP53" s="84"/>
+      <c r="CQ53" s="84"/>
+      <c r="CR53" s="84"/>
+      <c r="CS53" s="84"/>
+      <c r="CT53" s="84"/>
+      <c r="CW53" s="84"/>
+      <c r="CX53" s="84"/>
+    </row>
+    <row r="54" spans="1:133">
+      <c r="A54" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>128</v>
       </c>
-      <c r="C53">
+      <c r="C54">
         <v>10</v>
       </c>
-      <c r="E53">
+      <c r="E54">
         <v>10</v>
       </c>
-      <c r="CM53" s="82"/>
-      <c r="CQ53" s="16"/>
-      <c r="DA53" s="84"/>
-      <c r="DD53" s="84"/>
-      <c r="DE53" s="84"/>
-      <c r="DF53" s="84"/>
-      <c r="DG53" s="84"/>
-      <c r="DH53" s="84"/>
-      <c r="DK53" s="84"/>
-      <c r="DL53" s="84"/>
-    </row>
-    <row r="54" spans="1:133">
       <c r="CM54" s="82"/>
       <c r="CQ54" s="16"/>
+      <c r="DA54" s="84"/>
+      <c r="DD54" s="84"/>
+      <c r="DE54" s="84"/>
+      <c r="DF54" s="84"/>
+      <c r="DG54" s="84"/>
+      <c r="DH54" s="84"/>
+      <c r="DK54" s="84"/>
+      <c r="DL54" s="84"/>
     </row>
     <row r="55" spans="1:133">
-      <c r="A55" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B55" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="BA55" s="79"/>
-      <c r="BB55" s="79"/>
-      <c r="BC55" s="79"/>
-      <c r="BD55" s="80"/>
       <c r="CM55" s="82"/>
       <c r="CQ55" s="16"/>
-      <c r="DO55" s="79"/>
-      <c r="DP55" s="79"/>
-      <c r="DQ55" s="79"/>
-      <c r="DR55" s="79"/>
-      <c r="DS55" s="79"/>
-      <c r="DT55" s="79"/>
-      <c r="DU55" s="79"/>
-      <c r="DV55" s="79"/>
-      <c r="DW55" s="79"/>
-      <c r="DX55" s="79"/>
-      <c r="DY55" s="79"/>
-      <c r="DZ55" s="79"/>
-      <c r="EA55" s="79"/>
-      <c r="EB55" s="79"/>
-      <c r="EC55" s="79"/>
     </row>
     <row r="56" spans="1:133">
-      <c r="A56" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="B56" t="s">
-        <v>123</v>
-      </c>
-      <c r="C56">
-        <v>1</v>
-      </c>
-      <c r="E56">
-        <v>1</v>
-      </c>
-      <c r="AW56" s="83"/>
-      <c r="BA56" s="82"/>
+      <c r="A56" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="BA56" s="79"/>
+      <c r="BB56" s="79"/>
+      <c r="BC56" s="79"/>
+      <c r="BD56" s="80"/>
       <c r="CM56" s="82"/>
       <c r="CQ56" s="16"/>
+      <c r="DO56" s="79"/>
+      <c r="DP56" s="79"/>
+      <c r="DQ56" s="79"/>
+      <c r="DR56" s="79"/>
+      <c r="DS56" s="79"/>
+      <c r="DT56" s="79"/>
+      <c r="DU56" s="79"/>
+      <c r="DV56" s="79"/>
+      <c r="DW56" s="79"/>
+      <c r="DX56" s="79"/>
+      <c r="DY56" s="79"/>
+      <c r="DZ56" s="79"/>
+      <c r="EA56" s="79"/>
+      <c r="EB56" s="79"/>
+      <c r="EC56" s="79"/>
     </row>
     <row r="57" spans="1:133">
       <c r="A57" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B57" t="s">
-        <v>40</v>
+        <v>123</v>
       </c>
       <c r="C57">
         <v>1</v>
@@ -3763,16 +3789,17 @@
       <c r="E57">
         <v>1</v>
       </c>
+      <c r="AW57" s="83"/>
+      <c r="BA57" s="82"/>
       <c r="CM57" s="82"/>
       <c r="CQ57" s="16"/>
-      <c r="DS57" s="83"/>
     </row>
     <row r="58" spans="1:133">
       <c r="A58" s="1" t="s">
-        <v>124</v>
+        <v>101</v>
       </c>
       <c r="B58" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -3782,11 +3809,24 @@
       </c>
       <c r="CM58" s="82"/>
       <c r="CQ58" s="16"/>
-      <c r="DZ58" s="83"/>
+      <c r="DS58" s="83"/>
     </row>
     <row r="59" spans="1:133">
+      <c r="A59" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B59" t="s">
+        <v>41</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>1</v>
+      </c>
       <c r="CM59" s="82"/>
       <c r="CQ59" s="16"/>
+      <c r="DZ59" s="83"/>
     </row>
     <row r="60" spans="1:133">
       <c r="CM60" s="82"/>
@@ -3813,42 +3853,42 @@
       <c r="CQ65" s="16"/>
     </row>
     <row r="66" spans="3:95">
-      <c r="C66">
-        <f>SUM(C4:C65)</f>
-        <v>297</v>
-      </c>
-      <c r="D66">
-        <f>SUM(D4:D65)</f>
-        <v>37</v>
-      </c>
-      <c r="E66" s="81">
-        <f>SUM(E4:E65)</f>
-        <v>303</v>
-      </c>
-      <c r="F66">
-        <f>SUM(F4:F65)</f>
-        <v>44</v>
-      </c>
       <c r="CM66" s="82"/>
       <c r="CQ66" s="16"/>
     </row>
     <row r="67" spans="3:95">
-      <c r="C67" t="s">
-        <v>102</v>
-      </c>
-      <c r="D67" t="s">
-        <v>103</v>
-      </c>
-      <c r="E67" t="s">
-        <v>130</v>
-      </c>
-      <c r="F67" t="s">
-        <v>129</v>
+      <c r="C67">
+        <f>SUM(C4:C66)</f>
+        <v>297</v>
+      </c>
+      <c r="D67">
+        <f>SUM(D4:D66)</f>
+        <v>37</v>
+      </c>
+      <c r="E67" s="81">
+        <f>SUM(E4:E66)</f>
+        <v>303</v>
+      </c>
+      <c r="F67">
+        <f>SUM(F4:F66)</f>
+        <v>44</v>
       </c>
       <c r="CM67" s="82"/>
       <c r="CQ67" s="16"/>
     </row>
     <row r="68" spans="3:95">
+      <c r="C68" t="s">
+        <v>102</v>
+      </c>
+      <c r="D68" t="s">
+        <v>103</v>
+      </c>
+      <c r="E68" t="s">
+        <v>130</v>
+      </c>
+      <c r="F68" t="s">
+        <v>129</v>
+      </c>
       <c r="CM68" s="82"/>
       <c r="CQ68" s="16"/>
     </row>
@@ -3878,6 +3918,7 @@
     </row>
     <row r="75" spans="3:95">
       <c r="CM75" s="82"/>
+      <c r="CQ75" s="16"/>
     </row>
     <row r="76" spans="3:95">
       <c r="CM76" s="82"/>
@@ -4271,6 +4312,9 @@
     </row>
     <row r="206" spans="91:91">
       <c r="CM206" s="82"/>
+    </row>
+    <row r="207" spans="91:91">
+      <c r="CM207" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>